<commit_message>
Added legend and benchmark
</commit_message>
<xml_diff>
--- a/tutorial/media/study.xlsx
+++ b/tutorial/media/study.xlsx
@@ -3,11 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Tests Coverage" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Tests Code" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="SMLP benchmark" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr/>
   <extLst>
@@ -17,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
   <si>
     <t>N</t>
   </si>
@@ -103,9 +104,24 @@
     <t>MultiObjective3</t>
   </si>
   <si>
+    <t>Legend</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test name</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Impemented</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not implemented</t>
+  </si>
+  <si>
     <t>`</t>
   </si>
   <si>
+    <t xml:space="preserve"> Test inputs</t>
+  </si>
+  <si>
     <t xml:space="preserve">  GLPK</t>
   </si>
   <si>
@@ -158,6 +174,27 @@
   </si>
   <si>
     <t>pyomo/py/nsga3_mixed.py</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test code</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Runtime, seconds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Minimal distance - decision tree</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Minimal distance - polynom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All other metods together - python3.12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All other metods together - python3.14</t>
   </si>
 </sst>
 </file>
@@ -266,7 +303,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left style="none"/>
       <right style="none"/>
@@ -304,6 +341,19 @@
       </bottom>
       <diagonal style="none"/>
     </border>
+    <border>
+      <left style="none"/>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -311,7 +361,7 @@
     <xf fontId="2" fillId="3" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
     <xf fontId="3" fillId="4" borderId="1" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="43">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -354,6 +404,25 @@
     <xf fontId="1" fillId="2" borderId="0" numFmtId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf fontId="4" fillId="0" borderId="2" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="4" fillId="7" borderId="2" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="2" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="1" fillId="2" borderId="2" numFmtId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="2" fillId="3" borderId="2" numFmtId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="2" numFmtId="0" xfId="0" applyBorder="1"/>
+    <xf fontId="3" fillId="4" borderId="3" numFmtId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -389,6 +458,31 @@
     <xf fontId="7" fillId="2" borderId="2" numFmtId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf fontId="6" fillId="7" borderId="2" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="7" fillId="2" borderId="2" numFmtId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="8" fillId="3" borderId="2" numFmtId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf fontId="0" fillId="6" borderId="2" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="1" fillId="2" borderId="2" numFmtId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="6" borderId="2" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="1" fillId="2" borderId="2" numFmtId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf fontId="1" fillId="2" borderId="2" numFmtId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1424,9 +1518,33 @@
         <v>19</v>
       </c>
     </row>
+    <row r="15" ht="14.25">
+      <c r="B15" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" ht="14.25">
+      <c r="B16" s="16"/>
+      <c r="C16" s="17" t="s">
+        <v>30</v>
+      </c>
+    </row>
     <row r="17" ht="14.25">
+      <c r="B17" s="16"/>
+      <c r="C17" s="18" t="s">
+        <v>31</v>
+      </c>
       <c r="N17" t="s">
-        <v>28</v>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" ht="14.25">
+      <c r="B18" s="19"/>
+      <c r="C18" s="20" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1449,237 +1567,367 @@
     <col customWidth="1" min="1" max="1" width="3.421875"/>
     <col customWidth="1" min="2" max="2" width="12.28125"/>
     <col customWidth="1" min="3" max="3" width="32.140625"/>
-    <col customWidth="1" min="4" max="4" style="14" width="24.140625"/>
+    <col customWidth="1" min="4" max="4" style="21" width="24.140625"/>
     <col customWidth="1" min="5" max="5" width="22.140625"/>
     <col customWidth="1" min="6" max="6" width="17.140625"/>
     <col customWidth="1" min="7" max="7" width="13.00390625"/>
     <col customWidth="1" min="8" max="8" width="26.57421875"/>
     <col customWidth="1" min="9" max="9" width="19.00390625"/>
-    <col customWidth="1" min="10" max="10" style="14" width="19.28125"/>
+    <col customWidth="1" min="10" max="10" style="21" width="19.28125"/>
     <col customWidth="1" min="11" max="11" width="28.28125"/>
-    <col customWidth="1" min="12" max="12" style="15" width="29.00390625"/>
+    <col customWidth="1" min="12" max="12" style="22" width="29.00390625"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="H1" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="I1" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="J1" s="17" t="s">
+      <c r="G1" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="I1" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="K1" s="17" t="s">
+      <c r="K1" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="L1" s="17" t="s">
+      <c r="L1" s="24" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="16">
+      <c r="A2" s="23">
         <v>1</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="E2" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="F2" s="19"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
-      <c r="J2" s="21"/>
-      <c r="K2" s="21"/>
-      <c r="L2" s="21"/>
+      <c r="C2" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2" s="26"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
+      <c r="K2" s="28"/>
+      <c r="L2" s="28"/>
     </row>
     <row r="3" ht="42.75" customHeight="1">
-      <c r="A3" s="16">
+      <c r="A3" s="23">
         <f t="shared" ref="A3:A9" si="1">A2+1</f>
         <v>2</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="D3" s="23"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="25" t="s">
-        <v>35</v>
-      </c>
-      <c r="I3" s="21"/>
-      <c r="J3" s="25" t="s">
-        <v>36</v>
-      </c>
-      <c r="K3" s="21"/>
-      <c r="L3" s="21"/>
+      <c r="C3" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="30"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="I3" s="28"/>
+      <c r="J3" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="K3" s="28"/>
+      <c r="L3" s="28"/>
     </row>
     <row r="4">
-      <c r="A4" s="16">
+      <c r="A4" s="23">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="D4" s="23"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="24"/>
-      <c r="J4" s="24"/>
-      <c r="K4" s="21"/>
-      <c r="L4" s="21"/>
+      <c r="C4" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="30"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="31"/>
+      <c r="K4" s="28"/>
+      <c r="L4" s="28"/>
     </row>
     <row r="5">
-      <c r="A5" s="16">
+      <c r="A5" s="23">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="24"/>
-      <c r="D5" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="E5" s="24"/>
-      <c r="F5" s="24"/>
-      <c r="G5" s="24"/>
-      <c r="H5" s="24"/>
-      <c r="I5" s="24"/>
-      <c r="J5" s="24"/>
-      <c r="K5" s="21"/>
-      <c r="L5" s="21"/>
-    </row>
-    <row r="6" ht="25.5">
-      <c r="A6" s="16">
+      <c r="C5" s="31"/>
+      <c r="D5" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="E5" s="31"/>
+      <c r="F5" s="31"/>
+      <c r="G5" s="31"/>
+      <c r="H5" s="31"/>
+      <c r="I5" s="31"/>
+      <c r="J5" s="31"/>
+      <c r="K5" s="28"/>
+      <c r="L5" s="28"/>
+    </row>
+    <row r="6" ht="22.5">
+      <c r="A6" s="23">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="26" t="s">
-        <v>40</v>
-      </c>
-      <c r="D6" s="23"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="24"/>
-      <c r="I6" s="24"/>
-      <c r="J6" s="24"/>
-      <c r="K6" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="L6" s="25" t="s">
-        <v>42</v>
+      <c r="C6" s="33" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" s="30"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="31"/>
+      <c r="G6" s="31"/>
+      <c r="H6" s="31"/>
+      <c r="I6" s="31"/>
+      <c r="J6" s="31"/>
+      <c r="K6" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="L6" s="32" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="16">
+      <c r="A7" s="23">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="24"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="24"/>
-      <c r="F7" s="24"/>
-      <c r="G7" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="H7" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="I7" s="24"/>
-      <c r="J7" s="24"/>
-      <c r="K7" s="21"/>
-      <c r="L7" s="21"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="H7" s="29" t="s">
+        <v>49</v>
+      </c>
+      <c r="I7" s="31"/>
+      <c r="J7" s="31"/>
+      <c r="K7" s="28"/>
+      <c r="L7" s="28"/>
     </row>
     <row r="8">
-      <c r="A8" s="16">
+      <c r="A8" s="23">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="24"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="24"/>
-      <c r="H8" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="I8" s="24"/>
-      <c r="J8" s="24"/>
-      <c r="K8" s="21"/>
-      <c r="L8" s="21"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="31"/>
+      <c r="G8" s="31"/>
+      <c r="H8" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="I8" s="31"/>
+      <c r="J8" s="31"/>
+      <c r="K8" s="28"/>
+      <c r="L8" s="28"/>
     </row>
     <row r="9">
-      <c r="A9" s="16">
+      <c r="A9" s="23">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="24"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="24"/>
-      <c r="F9" s="24"/>
-      <c r="G9" s="24"/>
-      <c r="H9" s="21"/>
-      <c r="I9" s="22" t="s">
-        <v>46</v>
-      </c>
-      <c r="J9" s="24"/>
-      <c r="K9" s="21"/>
-      <c r="L9" s="21"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="31"/>
+      <c r="G9" s="31"/>
+      <c r="H9" s="28"/>
+      <c r="I9" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="J9" s="31"/>
+      <c r="K9" s="28"/>
+      <c r="L9" s="28"/>
+    </row>
+    <row r="14" ht="14.25">
+      <c r="B14" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="34" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" ht="14.25">
+      <c r="B15" s="16"/>
+      <c r="C15" s="35" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" ht="14.25">
+      <c r="B16" s="16"/>
+      <c r="C16" s="36" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+  <sheetViews>
+    <sheetView zoomScale="100" workbookViewId="0">
+      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" style="1" width="4.421875"/>
+    <col customWidth="1" min="2" max="2" style="37" width="35.140625"/>
+    <col customWidth="1" min="3" max="3" width="18.28125"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="38">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="39">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="38">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="39">
+        <v>2330</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="38">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="39">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="38">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" s="39">
+        <v>5186</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="38">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6" s="39">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="40">
+        <v>6</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7" s="41">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="8" ht="14.25">
+      <c r="A8" s="40">
+        <v>7</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C8" s="42">
+        <v>619</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>

</xml_diff>